<commit_message>
upgrading so 1 excel file for all business types
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="3048" windowWidth="17280" windowHeight="8880" activeTab="1"/>
+    <workbookView xWindow="5316" yWindow="4392" windowWidth="17280" windowHeight="8880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Warmup" state="visible" r:id="rId4"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,9 @@
     <t>FollowUp</t>
   </si>
   <si>
+    <t>Campaign</t>
+  </si>
+  <si>
     <t>Lucas Aust</t>
   </si>
   <si>
@@ -62,7 +65,19 @@
     <t>CEO</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>landlord</t>
+  </si>
+  <si>
+    <t>ecommerce</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
@@ -467,7 +482,7 @@
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,10 +507,13 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -504,24 +522,117 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="14.4" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G3" t="s">
         <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="14.4" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" ht="14.4" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>